<commit_message>
updated ingredients and food tag matrix
</commit_message>
<xml_diff>
--- a/csv/Oisix/Demo_meals.xlsx
+++ b/csv/Oisix/Demo_meals.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunnyjones/Documents/Github/Saana_devel/csv/Oisix/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{364B970C-C1F5-1340-BE5E-6C5D88570FB5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF16F36-9765-B743-9D42-FAABA0344E5C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24720" windowHeight="17540" activeTab="3" xr2:uid="{E8325D28-9BCC-284E-A723-7EDFB092BAC9}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="17540" xr2:uid="{E8325D28-9BCC-284E-A723-7EDFB092BAC9}"/>
   </bookViews>
   <sheets>
     <sheet name="demo_ingredients" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="433">
   <si>
     <t>Item Name</t>
   </si>
@@ -1523,6 +1523,9 @@
   </si>
   <si>
     <t xml:space="preserve">Seaweed, Boiled hijiki </t>
+  </si>
+  <si>
+    <t>Shiitake mushroom</t>
   </si>
 </sst>
 </file>
@@ -2030,8 +2033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4490E09-7461-C04A-BE69-A23329171A10}">
   <dimension ref="A1:A572"/>
   <sheetViews>
-    <sheetView topLeftCell="A126" workbookViewId="0">
-      <selection activeCell="A143" sqref="A143"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -2056,7 +2059,7 @@
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="3" t="s">
-        <v>313</v>
+        <v>432</v>
       </c>
     </row>
     <row r="5" spans="1:1">
@@ -8716,7 +8719,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DDEC62F-35BD-AF4B-9125-14516A9A2331}">
   <dimension ref="A1:C76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>

</xml_diff>